<commit_message>
test fail snapshot test
</commit_message>
<xml_diff>
--- a/src/test/resources/GoyaNegLoginData.xlsx
+++ b/src/test/resources/GoyaNegLoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C21A393-A1C7-4436-8C09-58C9A83B00DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3606253-053B-4990-925F-4030A967A7D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -41,16 +41,25 @@
   </si>
   <si>
     <t>Pwd1@salesauthor1</t>
+  </si>
+  <si>
+    <t>test fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -382,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -394,7 +403,7 @@
     <col min="2" max="2" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,7 +411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -410,7 +419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -418,7 +427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -426,23 +435,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -450,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -458,19 +479,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>